<commit_message>
E2E for imagenet: design 1&2 works, 3 todo.
</commit_message>
<xml_diff>
--- a/end_to_end.xlsx
+++ b/end_to_end.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -443,105 +443,34 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>counts_r1</t>
+          <t>0.016650717703349284</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>counts_r5</t>
+          <t>0.00616267942583732</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>counts_r10</t>
+          <t>0.003827751196172249</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>counts_r20</t>
+          <t>0.0022870813397129187</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>counts_r30</t>
+          <t>0.0018883572567783093</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>counts_r1</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>counts_r5</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>counts_r10</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>counts_r20</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>counts_r30</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>0.04784688995215311</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>0.024727272727272726</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>0.015578947368421053</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>0.008688995215311005</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>0.006149920255183413</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>0.04784688995215311</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>0.024727272727272726</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>0.015578947368421053</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>0.008688995215311005</t>
-        </is>
-      </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>0.006149920255183413</t>
-        </is>
+      <c r="F1" t="n">
+        <v>30</v>
+      </c>
+      <c r="G1" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>